<commit_message>
fix use cases doc
</commit_message>
<xml_diff>
--- a/doc/Scenari/Invia email registrazione.xlsx
+++ b/doc/Scenari/Invia email registrazione.xlsx
@@ -33,9 +33,6 @@
     <t>Attori secondari</t>
   </si>
   <si>
-    <t>Nessuno</t>
-  </si>
-  <si>
     <t>Pre-condizione</t>
   </si>
   <si>
@@ -67,6 +64,9 @@
   </si>
   <si>
     <t>Il database contiene la nuova informazione inerente al token di registrazione che l'utente dovrà usare per confermare la registrazione.</t>
+  </si>
+  <si>
+    <t>Servizio di posta elettronica</t>
   </si>
 </sst>
 </file>
@@ -483,7 +483,7 @@
   <dimension ref="J9:K17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9:K17"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -497,7 +497,7 @@
         <v>0</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="10:11" x14ac:dyDescent="0.25">
@@ -505,7 +505,7 @@
         <v>1</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="10:11" ht="30" x14ac:dyDescent="0.25">
@@ -513,7 +513,7 @@
         <v>2</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="10:11" x14ac:dyDescent="0.25">
@@ -521,7 +521,7 @@
         <v>3</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="10:11" x14ac:dyDescent="0.25">
@@ -529,37 +529,37 @@
         <v>4</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="10:11" ht="30" x14ac:dyDescent="0.25">
       <c r="J14" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K14" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="10:11" ht="45" x14ac:dyDescent="0.25">
       <c r="J15" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="K15" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="10:11" ht="30" x14ac:dyDescent="0.25">
       <c r="J16" s="7"/>
       <c r="K16" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="10:11" ht="45" x14ac:dyDescent="0.25">
       <c r="J17" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K17" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>